<commit_message>
i311--lse eit2 extra suite file added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/others/linux_LSE_engine_sim.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/others/linux_LSE_engine_sim.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\TMP_EIT_suites\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0sngsN6DrFUqmuDZZhkIhd0EivD5xjZ0nj5fkMPZg+GIws2dGdQ895P+5SBGWtagLIQbEIRaHiBSjM2rhskk/Q==" workbookSaltValue="j22CHco5Hi8vlbKkcb9mlg==" workbookSpinCount="100000" lockStructure="1"/>
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1465,9 +1465,6 @@
     <t>synthesis</t>
   </si>
   <si>
-    <t>cmd = --devkit=jd5d80-7BG484I</t>
-  </si>
-  <si>
     <t>87</t>
   </si>
   <si>
@@ -1604,6 +1601,9 @@
   </si>
   <si>
     <t>radiant=ng2_3;questasim=10.6</t>
+  </si>
+  <si>
+    <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
   </si>
 </sst>
 </file>
@@ -5455,8 +5455,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{30096416-78A0-42B1-B12F-E1ED0B7E8601}" diskRevisions="1" revisionId="1194" version="15">
-  <header guid="{30096416-78A0-42B1-B12F-E1ED0B7E8601}" dateTime="2020-08-21T17:43:51" maxSheetId="5" userName="Jason Wang" r:id="rId15" minRId="1194">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E171EDB9-CFB9-459D-8CD9-876AFD349615}" diskRevisions="1" revisionId="1494" version="21">
+  <header guid="{E171EDB9-CFB9-459D-8CD9-876AFD349615}" dateTime="2020-11-02T08:47:57" maxSheetId="5" userName="Jason Wang" r:id="rId21" minRId="1326" maxRId="1493">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -5467,20 +5467,1530 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1194" sId="1">
+  <rcc rId="1326" sId="2">
+    <oc r="O130" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O130" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1327" sId="2">
+    <oc r="O129" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O129" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1328" sId="2">
+    <oc r="O89" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O89" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1329" sId="2">
+    <oc r="O90" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O90" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1330" sId="2">
+    <oc r="O91" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O91" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1331" sId="2">
+    <oc r="O92" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O92" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1332" sId="2">
+    <oc r="O93" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O93" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1333" sId="2">
+    <oc r="O94" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O94" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1334" sId="2">
+    <oc r="O95" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O95" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1335" sId="2">
+    <oc r="O96" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O96" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1336" sId="2">
+    <oc r="O97" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O97" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1337" sId="2">
+    <oc r="O98" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O98" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1338" sId="2">
+    <oc r="O99" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O99" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1339" sId="2">
+    <oc r="O100" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O100" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1340" sId="2">
+    <oc r="O101" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O101" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1341" sId="2">
+    <oc r="O102" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O102" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1342" sId="2">
+    <oc r="O103" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O103" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1343" sId="2">
+    <oc r="O104" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O104" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1344" sId="2">
+    <oc r="O105" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O105" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1345" sId="2">
+    <oc r="O106" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O106" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1346" sId="2">
+    <oc r="O107" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O107" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1347" sId="2">
+    <oc r="O108" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O108" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1348" sId="2">
+    <oc r="O109" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O109" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1349" sId="2">
+    <oc r="O110" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O110" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1350" sId="2">
+    <oc r="O111" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O111" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1351" sId="2">
+    <oc r="O112" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O112" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1352" sId="2">
+    <oc r="O113" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O113" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1353" sId="2">
+    <oc r="O114" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O114" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1354" sId="2">
+    <oc r="O115" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O115" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1355" sId="2">
+    <oc r="O116" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O116" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1356" sId="2">
+    <oc r="O117" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O117" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1357" sId="2">
+    <oc r="O118" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O118" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1358" sId="2">
+    <oc r="O119" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O119" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1359" sId="2">
+    <oc r="O120" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O120" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1360" sId="2">
+    <oc r="O121" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O121" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1361" sId="2">
+    <oc r="O122" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O122" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1362" sId="2">
+    <oc r="O123" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O123" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1363" sId="2">
+    <oc r="O124" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O124" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1364" sId="2">
+    <oc r="O125" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O125" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1365" sId="2">
+    <oc r="O126" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O126" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1366" sId="2">
+    <oc r="O127" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O127" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1367" sId="2">
+    <oc r="O128" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=jd5d80-7BG484I</t>
+      </is>
+    </oc>
+    <nc r="O128" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LFCPNX-100-7BBG484C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1368" sId="2">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B3"/>
+  </rcc>
+  <rcc rId="1369" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B4"/>
+  </rcc>
+  <rcc rId="1370" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rcc rId="1371" sId="2">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+  <rcc rId="1372" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B7"/>
+  </rcc>
+  <rcc rId="1373" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B8"/>
+  </rcc>
+  <rcc rId="1374" sId="2">
     <oc r="B9" t="inlineStr">
       <is>
-        <t>os_type=windows</t>
+        <t>YES</t>
       </is>
     </oc>
     <nc r="B9"/>
   </rcc>
+  <rcc rId="1375" sId="2">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B10"/>
+  </rcc>
+  <rcc rId="1376" sId="2">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B11"/>
+  </rcc>
+  <rcc rId="1377" sId="2">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B12"/>
+  </rcc>
+  <rcc rId="1378" sId="2">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B13"/>
+  </rcc>
+  <rcc rId="1379" sId="2">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B14"/>
+  </rcc>
+  <rcc rId="1380" sId="2">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B15"/>
+  </rcc>
+  <rcc rId="1381" sId="2">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B16"/>
+  </rcc>
+  <rcc rId="1382" sId="2">
+    <oc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B17"/>
+  </rcc>
+  <rcc rId="1383" sId="2">
+    <oc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B18"/>
+  </rcc>
+  <rcc rId="1384" sId="2">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B19"/>
+  </rcc>
+  <rcc rId="1385" sId="2">
+    <oc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B20"/>
+  </rcc>
+  <rcc rId="1386" sId="2">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B21"/>
+  </rcc>
+  <rcc rId="1387" sId="2">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B22"/>
+  </rcc>
+  <rcc rId="1388" sId="2">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B23"/>
+  </rcc>
+  <rcc rId="1389" sId="2">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B24"/>
+  </rcc>
+  <rcc rId="1390" sId="2">
+    <oc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B25"/>
+  </rcc>
+  <rcc rId="1391" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B26"/>
+  </rcc>
+  <rcc rId="1392" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B27"/>
+  </rcc>
+  <rcc rId="1393" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B28"/>
+  </rcc>
+  <rcc rId="1394" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B29"/>
+  </rcc>
+  <rcc rId="1395" sId="2">
+    <oc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B30"/>
+  </rcc>
+  <rcc rId="1396" sId="2">
+    <oc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B31"/>
+  </rcc>
+  <rcc rId="1397" sId="2">
+    <oc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B32"/>
+  </rcc>
+  <rcc rId="1398" sId="2">
+    <oc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B33"/>
+  </rcc>
+  <rcc rId="1399" sId="2">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="1400" sId="2">
+    <oc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B35"/>
+  </rcc>
+  <rcc rId="1401" sId="2">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="1402" sId="2">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="1403" sId="2">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="1404" sId="2">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="1405" sId="2">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+  <rcc rId="1406" sId="2">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B41"/>
+  </rcc>
+  <rcc rId="1407" sId="2">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B42"/>
+  </rcc>
+  <rcc rId="1408" sId="2">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B43"/>
+  </rcc>
+  <rcc rId="1409" sId="2">
+    <oc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B44"/>
+  </rcc>
+  <rcc rId="1410" sId="2">
+    <oc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B45"/>
+  </rcc>
+  <rcc rId="1411" sId="2">
+    <oc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B46"/>
+  </rcc>
+  <rcc rId="1412" sId="2">
+    <oc r="B47" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B47"/>
+  </rcc>
+  <rcc rId="1413" sId="2">
+    <oc r="B48" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B48"/>
+  </rcc>
+  <rcc rId="1414" sId="2">
+    <oc r="B49" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B49"/>
+  </rcc>
+  <rcc rId="1415" sId="2">
+    <oc r="B50" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B50"/>
+  </rcc>
+  <rcc rId="1416" sId="2">
+    <oc r="B51" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B51"/>
+  </rcc>
+  <rcc rId="1417" sId="2">
+    <oc r="B52" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B52"/>
+  </rcc>
+  <rcc rId="1418" sId="2">
+    <oc r="B53" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B53"/>
+  </rcc>
+  <rcc rId="1419" sId="2">
+    <oc r="B54" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B54"/>
+  </rcc>
+  <rcc rId="1420" sId="2">
+    <oc r="B55" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B55"/>
+  </rcc>
+  <rcc rId="1421" sId="2">
+    <oc r="B56" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B56"/>
+  </rcc>
+  <rcc rId="1422" sId="2">
+    <oc r="B57" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B57"/>
+  </rcc>
+  <rcc rId="1423" sId="2">
+    <oc r="B58" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B58"/>
+  </rcc>
+  <rcc rId="1424" sId="2">
+    <oc r="B59" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B59"/>
+  </rcc>
+  <rcc rId="1425" sId="2">
+    <oc r="B60" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B60"/>
+  </rcc>
+  <rcc rId="1426" sId="2">
+    <oc r="B61" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B61"/>
+  </rcc>
+  <rcc rId="1427" sId="2">
+    <oc r="B62" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B62"/>
+  </rcc>
+  <rcc rId="1428" sId="2">
+    <oc r="B63" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B63"/>
+  </rcc>
+  <rcc rId="1429" sId="2">
+    <oc r="B64" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B64"/>
+  </rcc>
+  <rcc rId="1430" sId="2">
+    <oc r="B65" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B65"/>
+  </rcc>
+  <rcc rId="1431" sId="2">
+    <oc r="B66" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B66"/>
+  </rcc>
+  <rcc rId="1432" sId="2">
+    <oc r="B67" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B67"/>
+  </rcc>
+  <rcc rId="1433" sId="2">
+    <oc r="B68" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B68"/>
+  </rcc>
+  <rcc rId="1434" sId="2">
+    <oc r="B69" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B69"/>
+  </rcc>
+  <rcc rId="1435" sId="2">
+    <oc r="B70" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B70"/>
+  </rcc>
+  <rcc rId="1436" sId="2">
+    <oc r="B71" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B71"/>
+  </rcc>
+  <rcc rId="1437" sId="2">
+    <oc r="B72" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B72"/>
+  </rcc>
+  <rcc rId="1438" sId="2">
+    <oc r="B73" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B73"/>
+  </rcc>
+  <rcc rId="1439" sId="2">
+    <oc r="B74" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B74"/>
+  </rcc>
+  <rcc rId="1440" sId="2">
+    <oc r="B75" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B75"/>
+  </rcc>
+  <rcc rId="1441" sId="2">
+    <oc r="B76" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B76"/>
+  </rcc>
+  <rcc rId="1442" sId="2">
+    <oc r="B77" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B77"/>
+  </rcc>
+  <rcc rId="1443" sId="2">
+    <oc r="B78" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B78"/>
+  </rcc>
+  <rcc rId="1444" sId="2">
+    <oc r="B79" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B79"/>
+  </rcc>
+  <rcc rId="1445" sId="2">
+    <oc r="B80" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B80"/>
+  </rcc>
+  <rcc rId="1446" sId="2">
+    <oc r="B81" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B81"/>
+  </rcc>
+  <rcc rId="1447" sId="2">
+    <oc r="B82" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B82"/>
+  </rcc>
+  <rcc rId="1448" sId="2">
+    <oc r="B83" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B83"/>
+  </rcc>
+  <rcc rId="1449" sId="2">
+    <oc r="B84" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B84"/>
+  </rcc>
+  <rcc rId="1450" sId="2">
+    <oc r="B85" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B85"/>
+  </rcc>
+  <rcc rId="1451" sId="2">
+    <oc r="B86" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B86"/>
+  </rcc>
+  <rcc rId="1452" sId="2">
+    <oc r="B87" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B87"/>
+  </rcc>
+  <rcc rId="1453" sId="2">
+    <oc r="B88" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B88"/>
+  </rcc>
+  <rcc rId="1454" sId="2">
+    <oc r="B89" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B89"/>
+  </rcc>
+  <rcc rId="1455" sId="2">
+    <oc r="B90" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B90"/>
+  </rcc>
+  <rcc rId="1456" sId="2">
+    <oc r="B91" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B91"/>
+  </rcc>
+  <rcc rId="1457" sId="2">
+    <oc r="B92" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B92"/>
+  </rcc>
+  <rcc rId="1458" sId="2">
+    <oc r="B93" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B93"/>
+  </rcc>
+  <rcc rId="1459" sId="2">
+    <oc r="B94" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B94"/>
+  </rcc>
+  <rcc rId="1460" sId="2">
+    <oc r="B95" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B95"/>
+  </rcc>
+  <rcc rId="1461" sId="2">
+    <oc r="B96" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B96"/>
+  </rcc>
+  <rcc rId="1462" sId="2">
+    <oc r="B97" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B97"/>
+  </rcc>
+  <rcc rId="1463" sId="2">
+    <oc r="B98" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B98"/>
+  </rcc>
+  <rcc rId="1464" sId="2">
+    <oc r="B99" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B99"/>
+  </rcc>
+  <rcc rId="1465" sId="2">
+    <oc r="B100" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B100"/>
+  </rcc>
+  <rcc rId="1466" sId="2">
+    <oc r="B101" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B101"/>
+  </rcc>
+  <rcc rId="1467" sId="2">
+    <oc r="B102" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B102"/>
+  </rcc>
+  <rcc rId="1468" sId="2">
+    <oc r="B103" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B103"/>
+  </rcc>
+  <rcc rId="1469" sId="2">
+    <oc r="B104" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B104"/>
+  </rcc>
+  <rcc rId="1470" sId="2">
+    <oc r="B105" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B105"/>
+  </rcc>
+  <rcc rId="1471" sId="2">
+    <oc r="B106" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B106"/>
+  </rcc>
+  <rcc rId="1472" sId="2">
+    <oc r="B107" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B107"/>
+  </rcc>
+  <rcc rId="1473" sId="2">
+    <oc r="B108" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B108"/>
+  </rcc>
+  <rcc rId="1474" sId="2">
+    <oc r="B109" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B109"/>
+  </rcc>
+  <rcc rId="1475" sId="2">
+    <oc r="B110" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B110"/>
+  </rcc>
+  <rcc rId="1476" sId="2">
+    <oc r="B111" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B111"/>
+  </rcc>
+  <rcc rId="1477" sId="2">
+    <oc r="B112" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B112"/>
+  </rcc>
+  <rcc rId="1478" sId="2">
+    <oc r="B113" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B113"/>
+  </rcc>
+  <rcc rId="1479" sId="2">
+    <oc r="B114" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B114"/>
+  </rcc>
+  <rcc rId="1480" sId="2">
+    <oc r="B115" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B115"/>
+  </rcc>
+  <rcc rId="1481" sId="2">
+    <oc r="B116" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B116"/>
+  </rcc>
+  <rcc rId="1482" sId="2">
+    <oc r="B117" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B117"/>
+  </rcc>
+  <rcc rId="1483" sId="2">
+    <oc r="B118" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B118"/>
+  </rcc>
+  <rcc rId="1484" sId="2">
+    <oc r="B119" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B119"/>
+  </rcc>
+  <rcc rId="1485" sId="2">
+    <oc r="B120" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B120"/>
+  </rcc>
+  <rcc rId="1486" sId="2">
+    <oc r="B121" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B121"/>
+  </rcc>
+  <rcc rId="1487" sId="2">
+    <oc r="B122" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B122"/>
+  </rcc>
+  <rcc rId="1488" sId="2">
+    <oc r="B123" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B123"/>
+  </rcc>
+  <rcc rId="1489" sId="2">
+    <oc r="B124" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B124"/>
+  </rcc>
+  <rcc rId="1490" sId="2">
+    <oc r="B125" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B125"/>
+  </rcc>
+  <rcc rId="1491" sId="2">
+    <oc r="B126" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B126"/>
+  </rcc>
+  <rcc rId="1492" sId="2">
+    <oc r="B127" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B127"/>
+  </rcc>
+  <rcc rId="1493" sId="2">
+    <oc r="B128" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B128"/>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -5774,7 +7284,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5805,7 +7315,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5831,7 +7341,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5839,7 +7349,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5860,18 +7370,18 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5887,11 +7397,11 @@
   <dimension ref="A1:AD130"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G110" sqref="G110"/>
+      <selection pane="bottomRight" activeCell="O130" sqref="E130:O130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7515,16 +9025,16 @@
     </row>
     <row r="89" spans="1:19">
       <c r="A89" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>354</v>
       </c>
       <c r="O89" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S89" s="18" t="s">
         <v>401</v>
@@ -7532,16 +9042,16 @@
     </row>
     <row r="90" spans="1:19">
       <c r="A90" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E90" s="18" t="s">
         <v>356</v>
       </c>
       <c r="O90" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S90" s="18" t="s">
         <v>401</v>
@@ -7549,16 +9059,16 @@
     </row>
     <row r="91" spans="1:19">
       <c r="A91" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E91" s="18" t="s">
         <v>357</v>
       </c>
       <c r="O91" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S91" s="18" t="s">
         <v>401</v>
@@ -7566,16 +9076,16 @@
     </row>
     <row r="92" spans="1:19">
       <c r="A92" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E92" s="18" t="s">
         <v>358</v>
       </c>
       <c r="O92" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S92" s="18" t="s">
         <v>401</v>
@@ -7583,16 +9093,16 @@
     </row>
     <row r="93" spans="1:19">
       <c r="A93" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E93" s="18" t="s">
         <v>359</v>
       </c>
       <c r="O93" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S93" s="18" t="s">
         <v>401</v>
@@ -7600,16 +9110,16 @@
     </row>
     <row r="94" spans="1:19">
       <c r="A94" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E94" s="18" t="s">
         <v>360</v>
       </c>
       <c r="O94" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S94" s="18" t="s">
         <v>401</v>
@@ -7617,16 +9127,16 @@
     </row>
     <row r="95" spans="1:19">
       <c r="A95" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E95" s="18" t="s">
         <v>361</v>
       </c>
       <c r="O95" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S95" s="18" t="s">
         <v>401</v>
@@ -7634,16 +9144,16 @@
     </row>
     <row r="96" spans="1:19">
       <c r="A96" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E96" s="18" t="s">
         <v>362</v>
       </c>
       <c r="O96" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S96" s="18" t="s">
         <v>401</v>
@@ -7651,16 +9161,16 @@
     </row>
     <row r="97" spans="1:19">
       <c r="A97" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E97" s="18" t="s">
         <v>363</v>
       </c>
       <c r="O97" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S97" s="18" t="s">
         <v>401</v>
@@ -7668,16 +9178,16 @@
     </row>
     <row r="98" spans="1:19">
       <c r="A98" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E98" s="18" t="s">
         <v>365</v>
       </c>
       <c r="O98" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S98" s="18" t="s">
         <v>401</v>
@@ -7685,16 +9195,16 @@
     </row>
     <row r="99" spans="1:19">
       <c r="A99" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E99" s="18" t="s">
         <v>366</v>
       </c>
       <c r="O99" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S99" s="18" t="s">
         <v>401</v>
@@ -7702,16 +9212,16 @@
     </row>
     <row r="100" spans="1:19">
       <c r="A100" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E100" s="18" t="s">
         <v>367</v>
       </c>
       <c r="O100" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S100" s="18" t="s">
         <v>401</v>
@@ -7719,16 +9229,16 @@
     </row>
     <row r="101" spans="1:19">
       <c r="A101" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E101" s="18" t="s">
         <v>368</v>
       </c>
       <c r="O101" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S101" s="18" t="s">
         <v>401</v>
@@ -7736,16 +9246,16 @@
     </row>
     <row r="102" spans="1:19">
       <c r="A102" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E102" s="18" t="s">
         <v>369</v>
       </c>
       <c r="O102" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S102" s="18" t="s">
         <v>401</v>
@@ -7753,16 +9263,16 @@
     </row>
     <row r="103" spans="1:19">
       <c r="A103" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E103" s="18" t="s">
         <v>370</v>
       </c>
       <c r="O103" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S103" s="18" t="s">
         <v>401</v>
@@ -7770,16 +9280,16 @@
     </row>
     <row r="104" spans="1:19">
       <c r="A104" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E104" s="18" t="s">
         <v>371</v>
       </c>
       <c r="O104" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S104" s="18" t="s">
         <v>401</v>
@@ -7787,16 +9297,16 @@
     </row>
     <row r="105" spans="1:19">
       <c r="A105" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E105" s="18" t="s">
         <v>372</v>
       </c>
       <c r="O105" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S105" s="18" t="s">
         <v>401</v>
@@ -7804,16 +9314,16 @@
     </row>
     <row r="106" spans="1:19">
       <c r="A106" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E106" s="18" t="s">
         <v>373</v>
       </c>
       <c r="O106" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S106" s="18" t="s">
         <v>401</v>
@@ -7821,16 +9331,16 @@
     </row>
     <row r="107" spans="1:19">
       <c r="A107" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E107" s="18" t="s">
         <v>374</v>
       </c>
       <c r="O107" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S107" s="18" t="s">
         <v>401</v>
@@ -7838,16 +9348,16 @@
     </row>
     <row r="108" spans="1:19">
       <c r="A108" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E108" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O108" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S108" s="18" t="s">
         <v>401</v>
@@ -7855,16 +9365,16 @@
     </row>
     <row r="109" spans="1:19">
       <c r="A109" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E109" s="18" t="s">
         <v>376</v>
       </c>
       <c r="O109" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S109" s="18" t="s">
         <v>401</v>
@@ -7872,16 +9382,16 @@
     </row>
     <row r="110" spans="1:19">
       <c r="A110" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E110" s="18" t="s">
         <v>377</v>
       </c>
       <c r="O110" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S110" s="18" t="s">
         <v>401</v>
@@ -7889,16 +9399,16 @@
     </row>
     <row r="111" spans="1:19">
       <c r="A111" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E111" s="18" t="s">
         <v>378</v>
       </c>
       <c r="O111" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S111" s="18" t="s">
         <v>401</v>
@@ -7906,16 +9416,16 @@
     </row>
     <row r="112" spans="1:19">
       <c r="A112" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>379</v>
       </c>
       <c r="O112" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S112" s="18" t="s">
         <v>401</v>
@@ -7923,16 +9433,16 @@
     </row>
     <row r="113" spans="1:19">
       <c r="A113" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E113" s="18" t="s">
         <v>380</v>
       </c>
       <c r="O113" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S113" s="18" t="s">
         <v>401</v>
@@ -7940,16 +9450,16 @@
     </row>
     <row r="114" spans="1:19">
       <c r="A114" s="18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E114" s="18" t="s">
         <v>381</v>
       </c>
       <c r="O114" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S114" s="18" t="s">
         <v>401</v>
@@ -7957,16 +9467,16 @@
     </row>
     <row r="115" spans="1:19">
       <c r="A115" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E115" s="18" t="s">
         <v>382</v>
       </c>
       <c r="O115" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S115" s="18" t="s">
         <v>401</v>
@@ -7974,16 +9484,16 @@
     </row>
     <row r="116" spans="1:19">
       <c r="A116" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E116" s="18" t="s">
         <v>383</v>
       </c>
       <c r="O116" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S116" s="18" t="s">
         <v>401</v>
@@ -7991,16 +9501,16 @@
     </row>
     <row r="117" spans="1:19">
       <c r="A117" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E117" s="18" t="s">
         <v>384</v>
       </c>
       <c r="O117" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S117" s="18" t="s">
         <v>401</v>
@@ -8008,16 +9518,16 @@
     </row>
     <row r="118" spans="1:19">
       <c r="A118" s="18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E118" s="18" t="s">
         <v>385</v>
       </c>
       <c r="O118" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S118" s="18" t="s">
         <v>401</v>
@@ -8025,16 +9535,16 @@
     </row>
     <row r="119" spans="1:19">
       <c r="A119" s="18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D119" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E119" s="18" t="s">
         <v>386</v>
       </c>
       <c r="O119" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S119" s="18" t="s">
         <v>401</v>
@@ -8042,16 +9552,16 @@
     </row>
     <row r="120" spans="1:19">
       <c r="A120" s="18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E120" s="18" t="s">
         <v>387</v>
       </c>
       <c r="O120" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S120" s="18" t="s">
         <v>401</v>
@@ -8059,16 +9569,16 @@
     </row>
     <row r="121" spans="1:19">
       <c r="A121" s="18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D121" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E121" s="18" t="s">
         <v>388</v>
       </c>
       <c r="O121" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S121" s="18" t="s">
         <v>401</v>
@@ -8076,16 +9586,16 @@
     </row>
     <row r="122" spans="1:19">
       <c r="A122" s="18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E122" s="18" t="s">
         <v>389</v>
       </c>
       <c r="O122" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S122" s="18" t="s">
         <v>401</v>
@@ -8093,16 +9603,16 @@
     </row>
     <row r="123" spans="1:19">
       <c r="A123" s="18" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E123" s="18" t="s">
         <v>390</v>
       </c>
       <c r="O123" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S123" s="18" t="s">
         <v>401</v>
@@ -8110,16 +9620,16 @@
     </row>
     <row r="124" spans="1:19">
       <c r="A124" s="18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E124" s="18" t="s">
         <v>391</v>
       </c>
       <c r="O124" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S124" s="18" t="s">
         <v>401</v>
@@ -8127,16 +9637,16 @@
     </row>
     <row r="125" spans="1:19">
       <c r="A125" s="18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E125" s="18" t="s">
         <v>392</v>
       </c>
       <c r="O125" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S125" s="18" t="s">
         <v>401</v>
@@ -8144,16 +9654,16 @@
     </row>
     <row r="126" spans="1:19">
       <c r="A126" s="18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E126" s="18" t="s">
         <v>393</v>
       </c>
       <c r="O126" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S126" s="18" t="s">
         <v>401</v>
@@ -8161,16 +9671,16 @@
     </row>
     <row r="127" spans="1:19">
       <c r="A127" s="18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E127" s="18" t="s">
         <v>394</v>
       </c>
       <c r="O127" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S127" s="18" t="s">
         <v>401</v>
@@ -8178,16 +9688,16 @@
     </row>
     <row r="128" spans="1:19">
       <c r="A128" s="18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E128" s="18" t="s">
         <v>395</v>
       </c>
       <c r="O128" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S128" s="18" t="s">
         <v>401</v>
@@ -8195,16 +9705,16 @@
     </row>
     <row r="129" spans="1:19">
       <c r="A129" s="18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E129" s="18" t="s">
         <v>396</v>
       </c>
       <c r="O129" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S129" s="18" t="s">
         <v>401</v>
@@ -8212,16 +9722,16 @@
     </row>
     <row r="130" spans="1:19">
       <c r="A130" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="D130" s="18" t="s">
         <v>444</v>
-      </c>
-      <c r="D130" s="18" t="s">
-        <v>445</v>
       </c>
       <c r="E130" s="18" t="s">
         <v>397</v>
       </c>
       <c r="O130" s="18" t="s">
-        <v>402</v>
+        <v>448</v>
       </c>
       <c r="S130" s="18" t="s">
         <v>401</v>
@@ -8231,26 +9741,26 @@
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="A2:AD2"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:Y2"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D129" sqref="D129"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -10497,6 +12007,9 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10505,9 +12018,6 @@
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>